<commit_message>
Colored figures and added rf gain block
</commit_message>
<xml_diff>
--- a/Cost_Estimate_SolarTele.xlsx
+++ b/Cost_Estimate_SolarTele.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\filehost\evla\techdocs\RFI\coopshare\remynguyen\SolarTelescope-ASWA\Solar-Telescope-Redesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED2D95E-AC68-4B8C-968B-1A001C0D1E5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3286944C-4D18-498B-AEE8-04EE493061E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{CEE51DDE-1FC0-4F37-B228-20480DD76876}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>Model Number</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/stmicroelectronics/L7815ABV/1038268 </t>
+  </si>
+  <si>
+    <t>Large 3V Analog Panel Meter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/adafruit-industries-llc/3989/9770510 </t>
   </si>
 </sst>
 </file>
@@ -742,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D95F8A-DC41-4103-8882-8D27318627F6}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,7 +811,7 @@
         <v>0.47</v>
       </c>
       <c r="D3" s="6">
-        <f>B3*C3</f>
+        <f t="shared" ref="D3:D40" si="0">B3*C3</f>
         <v>0.94</v>
       </c>
       <c r="E3" s="11" t="s">
@@ -830,7 +836,7 @@
         <v>0.79</v>
       </c>
       <c r="D4" s="6">
-        <f>B4*C4</f>
+        <f t="shared" si="0"/>
         <v>1.58</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -855,7 +861,7 @@
         <v>0.1</v>
       </c>
       <c r="D5" s="6">
-        <f>B5*C5</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="E5" s="11" t="s">
@@ -880,7 +886,7 @@
         <v>0.1</v>
       </c>
       <c r="D6" s="6">
-        <f>B6*C6</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="E6" s="11" t="s">
@@ -905,7 +911,7 @@
         <v>1.73</v>
       </c>
       <c r="D7" s="6">
-        <f>B7*C7</f>
+        <f t="shared" si="0"/>
         <v>1.73</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -930,7 +936,7 @@
         <v>3.99</v>
       </c>
       <c r="D8" s="6">
-        <f>B8*C8</f>
+        <f t="shared" si="0"/>
         <v>23.94</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -955,7 +961,7 @@
         <v>0.1</v>
       </c>
       <c r="D9" s="6">
-        <f>B9*C9</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -980,7 +986,7 @@
         <v>0.66</v>
       </c>
       <c r="D10" s="6">
-        <f>B10*C10</f>
+        <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
       <c r="E10" s="11" t="s">
@@ -1005,7 +1011,7 @@
         <v>0.19</v>
       </c>
       <c r="D11" s="6">
-        <f>B11*C11</f>
+        <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -1030,7 +1036,7 @@
         <v>0.36</v>
       </c>
       <c r="D12" s="6">
-        <f>B12*C12</f>
+        <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -1055,7 +1061,7 @@
         <v>0.1</v>
       </c>
       <c r="D13" s="6">
-        <f>B13*C13</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -1080,7 +1086,7 @@
         <v>0.1</v>
       </c>
       <c r="D14" s="6">
-        <f>B14*C14</f>
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="E14" s="11" t="s">
@@ -1105,7 +1111,7 @@
         <v>2.1</v>
       </c>
       <c r="D15" s="6">
-        <f>B15*C15</f>
+        <f t="shared" si="0"/>
         <v>4.2</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -1130,7 +1136,7 @@
         <v>0.1</v>
       </c>
       <c r="D16" s="6">
-        <f>B16*C16</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
       <c r="E16" s="11" t="s">
@@ -1155,7 +1161,7 @@
         <v>0.77</v>
       </c>
       <c r="D17" s="6">
-        <f>B17*C17</f>
+        <f t="shared" si="0"/>
         <v>0.77</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -1180,7 +1186,7 @@
         <v>0.77</v>
       </c>
       <c r="D18" s="6">
-        <f>B18*C18</f>
+        <f t="shared" si="0"/>
         <v>0.77</v>
       </c>
       <c r="E18" s="11" t="s">
@@ -1205,7 +1211,7 @@
         <v>17.39</v>
       </c>
       <c r="D19" s="6">
-        <f>B19*C19</f>
+        <f t="shared" si="0"/>
         <v>17.39</v>
       </c>
       <c r="E19" s="11" t="s">
@@ -1230,7 +1236,7 @@
         <v>0.41</v>
       </c>
       <c r="D20" s="6">
-        <f>B20*C20</f>
+        <f t="shared" si="0"/>
         <v>0.41</v>
       </c>
       <c r="E20" s="11" t="s">
@@ -1249,19 +1255,27 @@
     <row r="21" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="5">
-        <v>0</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="D21" s="6">
-        <f>B21*C21</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="4"/>
+        <f t="shared" si="0"/>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="10">
+        <v>3989</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
@@ -1272,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="6">
-        <f>B22*C22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E22" s="11"/>
@@ -1289,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="6">
-        <f>B23*C23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E23" s="11"/>
@@ -1306,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="6">
-        <f>B24*C24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E24" s="11"/>
@@ -1323,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="6">
-        <f>B25*C25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E25" s="11"/>
@@ -1340,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="6">
-        <f>B26*C26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E26" s="11"/>
@@ -1357,7 +1371,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="6">
-        <f>B27*C27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E27" s="11"/>
@@ -1374,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="6">
-        <f>B28*C28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E28" s="11"/>
@@ -1391,7 +1405,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="6">
-        <f>B29*C29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E29" s="11"/>
@@ -1408,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="6">
-        <f>B30*C30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E30" s="11"/>
@@ -1425,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="6">
-        <f>B31*C31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E31" s="11"/>
@@ -1442,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="6">
-        <f>B32*C32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E32" s="11"/>
@@ -1459,7 +1473,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="6">
-        <f>B33*C33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E33" s="11"/>
@@ -1476,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="6">
-        <f>B34*C34</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E34" s="11"/>
@@ -1493,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="6">
-        <f>B35*C35</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E35" s="11"/>
@@ -1510,7 +1524,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="6">
-        <f>B36*C36</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E36" s="11"/>
@@ -1527,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="6">
-        <f>B37*C37</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E37" s="11"/>
@@ -1544,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="6">
-        <f>B38*C38</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E38" s="11"/>
@@ -1561,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="6">
-        <f>B39*C39</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E39" s="11"/>
@@ -1578,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="D40" s="6">
-        <f>B40*C40</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E40" s="11"/>
@@ -1594,7 +1608,7 @@
       </c>
       <c r="D41" s="8">
         <f>SUM(D3:D40)</f>
-        <v>53.840000000000011</v>
+        <v>63.790000000000006</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -1621,8 +1635,9 @@
     <hyperlink ref="H5" r:id="rId16" xr:uid="{86FD8197-B477-4F5F-8087-62AAECFDECA4}"/>
     <hyperlink ref="H4" r:id="rId17" xr:uid="{477B4C67-B74A-4050-B314-B1CBC15278B8}"/>
     <hyperlink ref="H3" r:id="rId18" xr:uid="{429E3324-35B4-4CB4-A066-D5B0E7875262}"/>
+    <hyperlink ref="H21" r:id="rId19" xr:uid="{FEA7C32E-F678-44D9-8F32-06F092EACDF9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>